<commit_message>
Add robust date extraction with chrono-node
- Install chrono-node for natural language date parsing
- Create dateExtractor.js utility with confidence scoring
- Filter out events with dates clearly in the PAST
- Keep events without dates (default to today per user preference)
- Track dateConfidence: 'high', 'medium', 'low', 'none' on each event
- Update ExaClient, SerperClient, TicketmasterClient to use new extractor
</commit_message>
<xml_diff>
--- a/data/whitelist.xlsx
+++ b/data/whitelist.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2068,9 +2068,23 @@
         <v>San Francisco</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>broadwayworld.com</v>
+      </c>
+      <c r="B120" t="str">
+        <v>theatre</v>
+      </c>
+      <c r="C120" t="str">
+        <v>** Cowell Theater at Fort Mason Center for Arts &amp; Culture</v>
+      </c>
+      <c r="D120" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D119"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D120"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix HTTP 500 error when using AI instructions box
- Add try-catch with fallback in custom AI instructions mode
- When Perplexity API fails, gracefully fall back to multi-provider search
- Add defensive checks in buildCustomEventPrompt for edge cases
- Add global error handler in main.tsx to catch external errors
- Add try-catch in Dashboard.tsx AI instructions onChange handler
- Updated whitelist with broadwayworld.com
</commit_message>
<xml_diff>
--- a/data/whitelist.xlsx
+++ b/data/whitelist.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2082,9 +2082,51 @@
         <v/>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>secretsanfrancisco.com</v>
+      </c>
+      <c r="B121" t="str">
+        <v>custom_search</v>
+      </c>
+      <c r="C121" t="str">
+        <v>Brava Theater Center</v>
+      </c>
+      <c r="D121" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>sfcv.org</v>
+      </c>
+      <c r="B122" t="str">
+        <v>music</v>
+      </c>
+      <c r="C122" t="str">
+        <v>Bing Concert Hall</v>
+      </c>
+      <c r="D122" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>shazam.com</v>
+      </c>
+      <c r="B123" t="str">
+        <v>music</v>
+      </c>
+      <c r="C123" t="str">
+        <v>Bing Concert Hall</v>
+      </c>
+      <c r="D123" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D120"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D123"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>